<commit_message>
[IMP] Fix paartner list report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
@@ -25,16 +25,16 @@
     <t xml:space="preserve">Partner Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Is Customer?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Supplier?</t>
+    <t xml:space="preserve">Is Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Supplier</t>
   </si>
   <si>
     <t xml:space="preserve">Partner Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Title+Name</t>
+    <t xml:space="preserve">Partner Name</t>
   </si>
   <si>
     <t xml:space="preserve">Street</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Account Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Bank number</t>
+    <t xml:space="preserve">Bank Name</t>
   </si>
   <si>
     <t xml:space="preserve">Account Owner name</t>
@@ -343,8 +343,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[IMP] Adjust partner detail report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
@@ -274,7 +274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,7 +296,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -308,6 +308,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -414,7 +418,7 @@
       <c r="G1" s="7"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
@@ -425,10 +429,10 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -436,10 +440,10 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -447,21 +451,21 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -469,10 +473,10 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -480,10 +484,10 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -494,115 +498,115 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="14" t="s">
+      <c r="P10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="14" t="s">
+      <c r="R10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="T10" s="14" t="s">
+      <c r="T10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="U10" s="14" t="s">
+      <c r="U10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="14" t="s">
+      <c r="V10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="W10" s="14" t="s">
+      <c r="W10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="X10" s="14" t="s">
+      <c r="X10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="14" t="s">
+      <c r="Y10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="Z10" s="14" t="s">
+      <c r="Z10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AA10" s="14" t="s">
+      <c r="AA10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AB10" s="14" t="s">
+      <c r="AB10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AC10" s="14" t="s">
+      <c r="AC10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AD10" s="14" t="s">
+      <c r="AD10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AE10" s="14" t="s">
+      <c r="AE10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AF10" s="14" t="s">
+      <c r="AF10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AG10" s="15" t="s">
+      <c r="AG10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AH10" s="15" t="s">
+      <c r="AH10" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AI10" s="15" t="s">
+      <c r="AI10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AJ10" s="15" t="s">
+      <c r="AJ10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AK10" s="15" t="s">
+      <c r="AK10" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -640,7 +644,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5"/>
+      <c r="A1" s="9"/>
       <c r="B1" s="6"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
@@ -649,7 +653,7 @@
       <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
@@ -660,10 +664,10 @@
       <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
@@ -671,10 +675,10 @@
       <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="0"/>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
@@ -682,10 +686,10 @@
       <c r="G4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="0"/>
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
@@ -693,10 +697,10 @@
       <c r="G5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="0"/>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
@@ -704,10 +708,10 @@
       <c r="G6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
@@ -715,10 +719,10 @@
       <c r="G7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
@@ -734,26 +738,26 @@
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
     </row>
-    <row r="10" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+    <row r="10" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="17" t="s">
         <v>35</v>
       </c>
       <c r="AMJ10" s="0"/>

</xml_diff>

<commit_message>
Edit receivable detail and Update UI partner detail
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Partner Detail Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t xml:space="preserve">Partner Detail Report</t>
   </si>
@@ -32,10 +32,7 @@
     <t xml:space="preserve">Active</t>
   </si>
   <si>
-    <t xml:space="preserve">Is Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Supplier</t>
+    <t xml:space="preserve">Partner’s</t>
   </si>
   <si>
     <t xml:space="preserve">Run By</t>
@@ -368,10 +365,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK10"/>
+  <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -476,7 +473,7 @@
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -484,130 +481,119 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="C9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="E9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="G9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="H9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="K9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="L9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="M9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="N9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="O9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="P9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="Q9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="R9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="15" t="s">
+      <c r="S9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="15" t="s">
+      <c r="T9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="T10" s="15" t="s">
+      <c r="U9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="U10" s="15" t="s">
+      <c r="V9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="15" t="s">
+      <c r="W9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="W10" s="15" t="s">
+      <c r="X9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="X10" s="15" t="s">
+      <c r="Y9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="15" t="s">
+      <c r="Z9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="Z10" s="15" t="s">
+      <c r="AA9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AA10" s="15" t="s">
+      <c r="AB9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AB10" s="15" t="s">
+      <c r="AC9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AC10" s="15" t="s">
+      <c r="AD9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AD10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE10" s="15" t="s">
+      <c r="AF9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AF10" s="15" t="s">
+      <c r="AG9" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="AG10" s="16" t="s">
+      <c r="AH9" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AH10" s="16" t="s">
+      <c r="AI9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AI10" s="16" t="s">
+      <c r="AJ9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AJ10" s="16" t="s">
+      <c r="AK9" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="AK10" s="16" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -626,10 +612,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ10"/>
+  <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -685,16 +671,16 @@
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
-      <c r="F5" s="0"/>
-      <c r="G5" s="0"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
@@ -711,7 +697,7 @@
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
@@ -719,48 +705,37 @@
       <c r="G7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="14"/>
+      <c r="A8" s="0"/>
+      <c r="B8" s="0"/>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0"/>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-      <c r="G9" s="0"/>
-    </row>
-    <row r="10" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
+    <row r="9" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="C9" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="E9" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="AMJ10" s="0"/>
+      <c r="G9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AMJ9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[IMP] Remove supplier invoice detail
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
@@ -80,10 +80,10 @@
     <t xml:space="preserve">Postcode</t>
   </si>
   <si>
-    <t xml:space="preserve">TaxID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Branch</t>
+    <t xml:space="preserve">Tax ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax Branch ID</t>
   </si>
   <si>
     <t xml:space="preserve">Mobile</t>

</xml_diff>

<commit_message>
[IMP] add fields clc and slc in partner detail report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t xml:space="preserve">Partner Detail Report</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Legacy Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Legacy Code</t>
   </si>
   <si>
     <t xml:space="preserve">Internal Note</t>
@@ -161,7 +167,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -208,6 +214,12 @@
       <name val="FreeSans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -286,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -351,15 +363,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -380,10 +396,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -400,24 +416,25 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="31.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="33.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="33.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="37.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="38.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="40.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="39.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="39.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="39.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="43.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="4" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="4" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="37.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="38.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="40.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="39.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="39.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="39.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="43.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="4" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="4" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="40" style="0" width="17.4"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -570,7 +587,7 @@
       <c r="T10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="U10" s="15" t="s">
+      <c r="U10" s="16" t="s">
         <v>26</v>
       </c>
       <c r="V10" s="15" t="s">
@@ -598,28 +615,34 @@
         <v>34</v>
       </c>
       <c r="AD10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AE10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG10" s="16" t="s">
+      <c r="AG10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AH10" s="16" t="s">
+      <c r="AH10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AI10" s="16" t="s">
+      <c r="AI10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="AJ10" s="16" t="s">
+      <c r="AJ10" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AK10" s="16" t="s">
+      <c r="AK10" s="17" t="s">
         <v>41</v>
+      </c>
+      <c r="AL10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM10" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -750,27 +773,27 @@
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
     </row>
-    <row r="10" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
+    <row r="10" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="C10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>35</v>
+      <c r="G10" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="AMJ10" s="0"/>
     </row>

</xml_diff>

<commit_message>
[IMP] Adjust partner detail
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_partner_detail.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t xml:space="preserve">Partner Detail Report</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">Partner Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is a Company?</t>
   </si>
   <si>
     <t xml:space="preserve">Customer</t>
@@ -167,7 +170,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,12 +217,6 @@
       <name val="FreeSans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -298,7 +295,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,7 +344,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,23 +364,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,45 +401,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AN10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="8" style="1" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="31.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="33.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="33.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="37.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="38.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="40.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="39.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="39.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="39.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="43.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="4" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="4" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="40" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="9" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="25.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="31.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="37.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="38.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="40.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="39.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="39.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="39.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="43.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="4" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="4" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="41" style="0" width="17.4"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -444,7 +450,8 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
@@ -455,194 +462,204 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="7"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="7"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="6"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="P10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="15" t="s">
+      <c r="R10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="15" t="s">
+      <c r="S10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="T10" s="15" t="s">
+      <c r="T10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="U10" s="16" t="s">
+      <c r="U10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="15" t="s">
+      <c r="V10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="W10" s="15" t="s">
+      <c r="W10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="X10" s="15" t="s">
+      <c r="X10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="15" t="s">
+      <c r="Y10" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="Z10" s="15" t="s">
+      <c r="Z10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AA10" s="15" t="s">
+      <c r="AA10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AB10" s="15" t="s">
+      <c r="AB10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AC10" s="15" t="s">
+      <c r="AC10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="AD10" s="15" t="s">
+      <c r="AD10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AE10" s="15" t="s">
+      <c r="AE10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="AF10" s="15" t="s">
+      <c r="AF10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="AG10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH10" s="15" t="s">
+      <c r="AH10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="AI10" s="17" t="s">
+      <c r="AI10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="AJ10" s="17" t="s">
+      <c r="AJ10" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AK10" s="17" t="s">
+      <c r="AK10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AL10" s="17" t="s">
+      <c r="AL10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AM10" s="17" t="s">
+      <c r="AM10" s="19" t="s">
         <v>43</v>
+      </c>
+      <c r="AN10" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -724,22 +741,22 @@
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,7 +774,7 @@
       <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
@@ -773,27 +790,27 @@
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
     </row>
-    <row r="10" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+    <row r="10" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="D10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="18" t="s">
-        <v>37</v>
+      <c r="G10" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="AMJ10" s="0"/>
     </row>

</xml_diff>